<commit_message>
20210901 1657 tlw8748253: EOD updates.
</commit_message>
<xml_diff>
--- a/docs/AMT.xlsx
+++ b/docs/AMT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Expense-Reimbursement-System\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw8748253\Desktop\Projects\Aromatic-Mountain-Technologies-BE\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC7F21D-30ED-48BB-B076-8304D33CE056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="5070" windowWidth="27465" windowHeight="9990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="470" yWindow="5070" windowWidth="27470" windowHeight="9990"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="149">
   <si>
     <t>Test Class</t>
   </si>
@@ -44,9 +43,6 @@
     <t>Test Description</t>
   </si>
   <si>
-    <t>Test Order</t>
-  </si>
-  <si>
     <t>PM Number</t>
   </si>
   <si>
@@ -84,9 +80,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Post Man</t>
   </si>
   <si>
     <t>/ers_login</t>
@@ -136,111 +129,9 @@
     </r>
   </si>
   <si>
-    <t>ERSAdminServiceTest</t>
-  </si>
-  <si>
     <t>ERSAdminService</t>
   </si>
   <si>
-    <t>addReimbursementStatus</t>
-  </si>
-  <si>
-    <t>Success added new Reimbursement status to database.</t>
-  </si>
-  <si>
-    <t>Expected: Exception adding duplicate Reimbursement status to database.</t>
-  </si>
-  <si>
-    <t>testAddReimbursementStatusDuplicate</t>
-  </si>
-  <si>
-    <t>testAddReimbursementStatusSuccess</t>
-  </si>
-  <si>
-    <t>testAddReimbursementStatusBadParamStatus</t>
-  </si>
-  <si>
-    <t>testAddReimbursementStatusBadParamStatusDesc</t>
-  </si>
-  <si>
-    <t>Expected: Exception adding bad parameter. Status less than 6.</t>
-  </si>
-  <si>
-    <t>Expected: Exception adding bad parameter. No Status Description.</t>
-  </si>
-  <si>
-    <t>testAddReimbursementTypeSuccess</t>
-  </si>
-  <si>
-    <t>testGetAllReimbursementStatusSuccess</t>
-  </si>
-  <si>
-    <t>testGetAllReimbursementStatusException</t>
-  </si>
-  <si>
-    <t>getAllReimbursementStatus</t>
-  </si>
-  <si>
-    <t>Success get all reimbursement statuses from the database.</t>
-  </si>
-  <si>
-    <t>Expected: Exception getting records from the database.</t>
-  </si>
-  <si>
-    <t>testGetAllReimbursementTypeSuccess</t>
-  </si>
-  <si>
-    <t>addReimbursementType</t>
-  </si>
-  <si>
-    <t>Success added new Reimbursement type to database.</t>
-  </si>
-  <si>
-    <t>getAllReimbursementType</t>
-  </si>
-  <si>
-    <t>Success get all reimbursement types from the database.</t>
-  </si>
-  <si>
-    <t>testAddUserRoleSuccess</t>
-  </si>
-  <si>
-    <t>addUserRole</t>
-  </si>
-  <si>
-    <t>Success added new User Role to database.</t>
-  </si>
-  <si>
-    <t>testGetAllUserRoleSuccess</t>
-  </si>
-  <si>
-    <t>getAllRecords</t>
-  </si>
-  <si>
-    <t>Success get all user roles from the database.</t>
-  </si>
-  <si>
-    <t>ERSService</t>
-  </si>
-  <si>
-    <t>test_addNewUserSuccess</t>
-  </si>
-  <si>
-    <t>ERSServiceTest</t>
-  </si>
-  <si>
-    <t>addNewUser</t>
-  </si>
-  <si>
-    <t>Success adding a user.</t>
-  </si>
-  <si>
-    <t>test_addNewUserBadPwdNoCapLetter</t>
-  </si>
-  <si>
-    <t>Expected: BadParameterException.  Logfile: password eror contains no capital letter.</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -368,12 +259,246 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>AdminService</t>
+  </si>
+  <si>
+    <t>test_AddAddressType_Success</t>
+  </si>
+  <si>
+    <t>addAddressType</t>
+  </si>
+  <si>
+    <t>test_AddAddressType_Exception</t>
+  </si>
+  <si>
+    <t>Exception service layer: BadParameterException: [Invalid Address Type parameters received.]</t>
+  </si>
+  <si>
+    <t>Additional Information</t>
+  </si>
+  <si>
+    <t>addAddressType(): Invalid parameters received sType: [TYPE_NOT_IN_LIST] sTypeDesc: [SHIPPING: The address where the customer wants the merchandise shipped.]</t>
+  </si>
+  <si>
+    <t>DatabaseException: [Error with database when adding Address Type.]</t>
+  </si>
+  <si>
+    <t>addAddressType(): Invalid parameters received sType: [] sTypeDesc: [SHIPPING: The address where the customer wants the merchandise shipped.]</t>
+  </si>
+  <si>
+    <t>addAddressType(): Invalid parameters received sType: [SHIPPING] sTypeDesc: []</t>
+  </si>
+  <si>
+    <t>addAddressType(): calling addRecord to add: objAddressTypeDTO: [[address_type]: [SHIPPING][address_type_desc]: [SHIPPING: The address where the customer wants the merchandise shipped.]]</t>
+  </si>
+  <si>
+    <t>test_AddAddressType_BadParam_Type_Not_In_List</t>
+  </si>
+  <si>
+    <t>test_AddAddressType_BadParam_Type_Blank</t>
+  </si>
+  <si>
+    <t>test_AddAddressType_BadParam_TypeDesc_Blank</t>
+  </si>
+  <si>
+    <t>test_AddCatalogItemType_Success</t>
+  </si>
+  <si>
+    <t>Success mock adding new record to database.</t>
+  </si>
+  <si>
+    <t>Exception mock adding new record to database.</t>
+  </si>
+  <si>
+    <t>addCatalogItemType</t>
+  </si>
+  <si>
+    <t>test_AddCatalogItemType_Exception</t>
+  </si>
+  <si>
+    <t>test_AddCatalogItemType_BadParam_Type_Not_In_List</t>
+  </si>
+  <si>
+    <t>test_AddCatalogItemType_BadParam_Type_Blank</t>
+  </si>
+  <si>
+    <t>test_AddCatalogItemType_BadParam_TypeDesc_Blank</t>
+  </si>
+  <si>
+    <t>DatabaseException: [Error with database when adding Catalog Item Type.]</t>
+  </si>
+  <si>
+    <t>addCatalogItemType(): calling addRecord to add: objTypeDTO: [[catalog_item_type]: [ACCESSORY][catalog_item_type_desc]: [ACCESSORY: coffee cups, makers, and other items related to coffee.]]</t>
+  </si>
+  <si>
+    <t>Exception service layer: BadParameterException: [Invalid Catalog Item Type parameters received.]</t>
+  </si>
+  <si>
+    <t>addCatalogItemType(): Invalid parameters received sType: [NOT_IN_LIST] sTypeDesc: [ACCESSORY: coffee cups, makers, and other items related to coffee.]</t>
+  </si>
+  <si>
+    <t>addCatalogItemType(): Invalid parameters received sType: [] sTypeDesc: [ACCESSORY: coffee cups, makers, and other items related to coffee.]</t>
+  </si>
+  <si>
+    <t>addCatalogItemType(): Invalid parameters received sType: [ACCESSORY] sTypeDesc: []</t>
+  </si>
+  <si>
+    <t>test_AddEmployeeRole_Success</t>
+  </si>
+  <si>
+    <t>test_AddEmployeeRole_Exception</t>
+  </si>
+  <si>
+    <t>test_AddEmployeeRole_BadParam_Type_Not_In_List</t>
+  </si>
+  <si>
+    <t>test_AddEmployeeRole_BadParam_Type_Blank</t>
+  </si>
+  <si>
+    <t>test_AddEmployeeRole_BadParam_TypeDesc_Blank</t>
+  </si>
+  <si>
+    <t>addEmployeeRole</t>
+  </si>
+  <si>
+    <t>Exception service layer: BadParameterException: [Invalid Employee Role parameters received.]</t>
+  </si>
+  <si>
+    <t>addUserRole(): calling addRecord to add: objEmployeeRoleDTO: [[employee_role]: [CATALOG_EMPLOYEE][employee_role_desc]: [CATALOG EMPLOYEE: A Catalog Employee creates catalog items and pages.]]</t>
+  </si>
+  <si>
+    <t>DatabaseException: [Error with database when adding Employee Role.]</t>
+  </si>
+  <si>
+    <t>addUserRole(): Invalid parameters received sRole: [NOT_IN_LIST] sRoleDesc: [CATALOG EMPLOYEE: A Catalog Employee creates catalog items and pages.]</t>
+  </si>
+  <si>
+    <t>addUserRole(): Invalid parameters received sRole: [] sRoleDesc: [CATALOG EMPLOYEE: A Catalog Employee creates catalog items and pages.]</t>
+  </si>
+  <si>
+    <t>addUserRole(): Invalid parameters received sRole: [CATALOG_EMPLOYEE] sRoleDesc: []</t>
+  </si>
+  <si>
+    <t>test_AddOrderStatus_Success</t>
+  </si>
+  <si>
+    <t>test_AddOrderStatus_Exception</t>
+  </si>
+  <si>
+    <t>test_AddOrderStatus_BadParam_Type_Not_In_List</t>
+  </si>
+  <si>
+    <t>test_AddOrderStatus_BadParam_Type_Blank</t>
+  </si>
+  <si>
+    <t>test_AddOrderStatus_BadParam_TypeDesc_Blank</t>
+  </si>
+  <si>
+    <t>addOrderStatus</t>
+  </si>
+  <si>
+    <t>addOrderStatus(): calling addRecord to add: objStatusDTO: [[order_status]: [PAID][order_status_desc]: [PAID: The order has been paid.]]</t>
+  </si>
+  <si>
+    <t>DatabaseException: [Error with database when adding Order Status.]</t>
+  </si>
+  <si>
+    <t>Exception service layer: BadParameterException: [Invalid Order Status parameters received.]</t>
+  </si>
+  <si>
+    <t>addOrderStatus(): Entered: objStatusDTO: [[order_status]: [NOT_IN_LIST][order_status_desc]: [PAID: The order has been paid.]]</t>
+  </si>
+  <si>
+    <t>addOrderStatus(): Invalid parameters received sStatus: [PAID] sStatusDesc: []</t>
+  </si>
+  <si>
+    <t>addOrderStatus(): Invalid parameters received sStatus: [] sStatusDesc: [PAID: The order has been paid.]</t>
+  </si>
+  <si>
+    <t>test_AddPhoneNumberType_Success</t>
+  </si>
+  <si>
+    <t>test_AddPhoneNumberType_Exception</t>
+  </si>
+  <si>
+    <t>test_AddPhoneNumberType_BadParam_Type_Not_In_List</t>
+  </si>
+  <si>
+    <t>test_AddPhoneNumberType_BadParam_Type_Blank</t>
+  </si>
+  <si>
+    <t>test_AddPhoneNumberType_BadParam_TypeDesc_Blank</t>
+  </si>
+  <si>
+    <t>addPhoneNumberType</t>
+  </si>
+  <si>
+    <t>addPhoneNumberType(): calling addRecord to add: objTypeDTO: [[phone_number_type]: [MOBILE][phone_number_type_desc]: [MOBILE: Phone number belongs to a mobile device.]]</t>
+  </si>
+  <si>
+    <t>DatabaseException: [Error with database when adding Phone Number Type.]</t>
+  </si>
+  <si>
+    <t>addPhoneNumberType(): Invalid Phone Number Type parameters received. sType: [NOT_IN_LIST] sTypeDesc: [MOBILE: Phone number belongs to a mobile device.]</t>
+  </si>
+  <si>
+    <t>addPhoneNumberType(): Invalid Phone Number Type parameters received. sType: [] sTypeDesc: [MOBILE: Phone number belongs to a mobile device.]</t>
+  </si>
+  <si>
+    <t>addPhoneNumberType(): Invalid Phone Number Type parameters received. sType: [MOBILE] sTypeDesc: []</t>
+  </si>
+  <si>
+    <t>Exception service layer: BadParameterException: [Invalid Phone Number Type parameters received.]</t>
+  </si>
+  <si>
+    <t>test_AddUserType_Success</t>
+  </si>
+  <si>
+    <t>addUserType</t>
+  </si>
+  <si>
+    <t>test_AddUserType_Exception</t>
+  </si>
+  <si>
+    <t>test_AddUserType_BadParam_Type_Not_In_List</t>
+  </si>
+  <si>
+    <t>test_AddUserType_BadParam_Type_Blank</t>
+  </si>
+  <si>
+    <t>test_AddUserType_BadParam_TypeDesc_Blank</t>
+  </si>
+  <si>
+    <t>addUserType(): calling addRecord to add: objUserTypeDTO: [[user_type]: [CUSTOMER][user_type_desc]: [CUSTOMER: This user type is an external customer viewing the catalog and buying merchandise.]]</t>
+  </si>
+  <si>
+    <t>DatabaseException: [Error with database when adding User Type.]</t>
+  </si>
+  <si>
+    <t>Exception service layer: BadParameterException: [Invalid User Type parameters received.]</t>
+  </si>
+  <si>
+    <t>addUserType(): Invalid User Type parameters received. sType: [NOT_IN_LIST] sTypeDesc: [CUSTOMER: This user type is an external customer viewing the catalog and buying merchandise.]</t>
+  </si>
+  <si>
+    <t>addUserType(): Invalid User Type parameters received. sType: [] sTypeDesc: [CUSTOMER: This user type is an external customer viewing the catalog and buying merchandise.]</t>
+  </si>
+  <si>
+    <t>addUserType(): Invalid User Type parameters received. sType: [CUSTOMER] sTypeDesc: []</t>
+  </si>
+  <si>
+    <t># of Cases</t>
+  </si>
+  <si>
+    <t>Test Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000.00"/>
     <numFmt numFmtId="165" formatCode="000.000"/>
@@ -502,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -590,6 +715,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -870,280 +1001,859 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="25"/>
+    <col min="1" max="1" width="9.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="141.26953125" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="37">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="28">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="37">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="28">
+        <v>1E-3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="37">
+        <f t="shared" ref="A4:A31" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="28">
+        <v>2E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="37">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="28">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="37">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="28">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="37">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="28">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="37">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="28">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="37">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="28">
+        <v>1.002</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="37">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="28">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="37">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="28">
+        <v>1.004</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="37">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="28">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="37">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="28">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="D13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="37">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="28">
+        <v>2.0019999999999998</v>
+      </c>
+      <c r="D14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="37">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="28">
+        <v>2.0030000000000001</v>
+      </c>
+      <c r="D15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="37">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="28">
+        <v>2.004</v>
+      </c>
+      <c r="D16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="37">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="28">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="37">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="28">
+        <v>3.0009999999999999</v>
+      </c>
+      <c r="D18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="37">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="28">
+        <v>3.0019999999999998</v>
+      </c>
+      <c r="D19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="37">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="28">
+        <v>3.0030000000000001</v>
+      </c>
+      <c r="D20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="37">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="28">
+        <v>3.004</v>
+      </c>
+      <c r="D21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="37">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="28">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="37">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="28">
+        <v>4.0010000000000003</v>
+      </c>
+      <c r="D23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>128</v>
+      </c>
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="37">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="28">
+        <v>4.0019999999999998</v>
+      </c>
+      <c r="D24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>128</v>
+      </c>
+      <c r="G24" t="s">
+        <v>134</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="37">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="28">
+        <v>4.0030000000000001</v>
+      </c>
+      <c r="D25" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" t="s">
+        <v>134</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="37">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="28">
+        <v>4.0039999999999996</v>
+      </c>
+      <c r="D26" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="37">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="28">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>136</v>
+      </c>
+      <c r="G27" t="s">
+        <v>86</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="37">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="28">
+        <v>5.0010000000000003</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G28" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="37">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="28">
+        <v>5.0019999999999998</v>
+      </c>
+      <c r="D29" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" t="s">
+        <v>143</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="37">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B2" s="28">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="28">
+        <v>5.0030000000000001</v>
+      </c>
+      <c r="D30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="37">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="28">
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="28">
-        <v>1.002</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="28">
-        <v>1.0029999999999999</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="28">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="28">
-        <v>2.0009999999999999</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="28">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="28">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="28">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="28">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="28">
-        <v>100</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="28">
-        <v>101</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s">
-        <v>63</v>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="28">
+        <v>5.0039999999999996</v>
+      </c>
+      <c r="D31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" t="s">
+        <v>136</v>
+      </c>
+      <c r="G31" t="s">
+        <v>143</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1153,7 +1863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1163,107 +1873,107 @@
       <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
     <col min="4" max="4" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="5" max="5" width="29.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>22</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="19"/>
@@ -1273,10 +1983,10 @@
       <c r="H4" s="18"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="19"/>
@@ -1286,10 +1996,10 @@
       <c r="H5" s="18"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="19"/>
@@ -1299,10 +2009,10 @@
       <c r="H6" s="18"/>
       <c r="I6" s="19"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="19"/>
@@ -1312,12 +2022,12 @@
       <c r="H7" s="18"/>
       <c r="I7" s="23"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="19"/>
@@ -1327,12 +2037,12 @@
       <c r="H8" s="18"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>10</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
@@ -1342,12 +2052,12 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
         <v>10.01</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="19"/>
@@ -1357,12 +2067,12 @@
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>10.02</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="19"/>
@@ -1372,12 +2082,12 @@
       <c r="H11" s="18"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>10.029999999999999</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="19"/>
@@ -1387,12 +2097,12 @@
       <c r="H12" s="18"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
         <v>15</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="19"/>
@@ -1402,12 +2112,12 @@
       <c r="H13" s="18"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>15.01</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="19"/>
@@ -1417,12 +2127,12 @@
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>15.02</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="19"/>
@@ -1432,12 +2142,12 @@
       <c r="H15" s="18"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>15.03</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19"/>
@@ -1447,12 +2157,12 @@
       <c r="H16" s="18"/>
       <c r="I16" s="21"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>20</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19"/>
@@ -1462,12 +2172,12 @@
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10">
         <v>20.010000000000002</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
@@ -1477,12 +2187,12 @@
       <c r="H18" s="18"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10">
         <v>20.02</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
@@ -1492,12 +2202,12 @@
       <c r="H19" s="18"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="10">
         <v>21</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19"/>
@@ -1507,12 +2217,12 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
         <v>21.01</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19"/>
@@ -1522,12 +2232,12 @@
       <c r="H21" s="18"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="10">
         <v>21.02</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19"/>
@@ -1537,12 +2247,12 @@
       <c r="H22" s="18"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="10">
         <v>25</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
@@ -1552,12 +2262,12 @@
       <c r="H23" s="18"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>25.01</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
@@ -1567,12 +2277,12 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="10">
         <v>25.02</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19"/>
@@ -1582,12 +2292,12 @@
       <c r="H25" s="18"/>
       <c r="I25" s="21"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="10">
         <v>25.03</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19"/>
@@ -1597,12 +2307,12 @@
       <c r="H26" s="18"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <v>25.04</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="19"/>
@@ -1612,12 +2322,12 @@
       <c r="H27" s="18"/>
       <c r="I27" s="21"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
         <v>0</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="19"/>
@@ -1627,12 +2337,12 @@
       <c r="H28" s="18"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="14">
         <v>0.01</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="19"/>
@@ -1642,12 +2352,12 @@
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="14">
         <v>0.02</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="19"/>
@@ -1657,12 +2367,12 @@
       <c r="H30" s="18"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="14">
         <v>0.03</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="19"/>
@@ -1672,12 +2382,12 @@
       <c r="H31" s="18"/>
       <c r="I31" s="21"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="14">
         <v>1</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="19"/>
@@ -1687,12 +2397,12 @@
       <c r="H32" s="18"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="14">
         <v>2</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="19"/>
@@ -1702,12 +2412,12 @@
       <c r="H33" s="18"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14">
         <v>5</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="19"/>
@@ -1717,12 +2427,12 @@
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14">
         <v>6</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="19"/>
@@ -1732,12 +2442,12 @@
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="14">
         <v>0</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="19"/>
@@ -1747,12 +2457,12 @@
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="14">
         <v>5</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="19"/>
@@ -1762,12 +2472,12 @@
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="10">
         <v>5.01</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="19"/>
@@ -1777,12 +2487,12 @@
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>0</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="19"/>
@@ -1792,12 +2502,12 @@
       <c r="H39" s="18"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="10">
         <v>0</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="19"/>
@@ -1807,12 +2517,12 @@
       <c r="H40" s="18"/>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="10">
         <v>5</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="19"/>
@@ -1822,12 +2532,12 @@
       <c r="H41" s="18"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
         <v>5</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="19"/>
@@ -1837,12 +2547,12 @@
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="10">
         <v>5.01</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
@@ -1852,7 +2562,7 @@
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="10"/>
       <c r="B44" s="13"/>
       <c r="C44" s="12"/>
@@ -1863,7 +2573,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="10"/>
       <c r="B45" s="13"/>
       <c r="C45" s="12"/>
@@ -1874,7 +2584,7 @@
       <c r="H45" s="12"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="10"/>
       <c r="B46" s="13"/>
       <c r="C46" s="12"/>
@@ -1885,7 +2595,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="10"/>
       <c r="B47" s="13"/>
       <c r="C47" s="12"/>
@@ -1896,7 +2606,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="10"/>
       <c r="B48" s="13"/>
       <c r="C48" s="12"/>
@@ -1907,7 +2617,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="10"/>
       <c r="B49" s="13"/>
       <c r="C49" s="12"/>
@@ -1918,7 +2628,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="10"/>
       <c r="B50" s="13"/>
       <c r="C50" s="12"/>
@@ -1929,7 +2639,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="10"/>
       <c r="B51" s="13"/>
       <c r="C51" s="12"/>
@@ -1940,7 +2650,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="10"/>
       <c r="B52" s="13"/>
       <c r="C52" s="12"/>
@@ -1951,7 +2661,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="10"/>
       <c r="B53" s="13"/>
       <c r="C53" s="12"/>
@@ -1962,7 +2672,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="10"/>
       <c r="B54" s="13"/>
       <c r="C54" s="12"/>
@@ -1973,7 +2683,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="10"/>
       <c r="B55" s="13"/>
       <c r="C55" s="12"/>
@@ -1984,7 +2694,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="10"/>
       <c r="B56" s="13"/>
       <c r="C56" s="12"/>
@@ -1995,7 +2705,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="10"/>
       <c r="B57" s="13"/>
       <c r="C57" s="12"/>
@@ -2006,7 +2716,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="10"/>
       <c r="B58" s="13"/>
       <c r="C58" s="12"/>
@@ -2017,7 +2727,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="10"/>
       <c r="B59" s="13"/>
       <c r="C59" s="12"/>
@@ -2028,7 +2738,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="10"/>
       <c r="B60" s="13"/>
       <c r="C60" s="12"/>
@@ -2039,7 +2749,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="10"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
@@ -2050,7 +2760,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="10"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
@@ -2061,7 +2771,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="10"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
@@ -2072,7 +2782,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="10"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
@@ -2083,7 +2793,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="10"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
@@ -2094,7 +2804,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="10"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
@@ -2112,428 +2822,428 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77A310-F525-46D4-AFD9-DE5E739D29B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" style="29" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="75.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7265625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="35.453125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
       <c r="G2" s="33" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="I2" s="34"/>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
       <c r="G3" s="33" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
       <c r="G4" s="33" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="I4" s="34"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
       <c r="G5" s="33" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="H5" s="34" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="I5" s="34"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="33" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="32"/>
       <c r="G6" s="32" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="33" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
       <c r="G7" s="32" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="I7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="33" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="35" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="I9" s="34"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="35" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="I10" s="34"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
       <c r="E11" s="33" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
       <c r="F12" s="33" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G12" s="32"/>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="33" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="33" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="33" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G15" s="32"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="33" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="33" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="E18" s="33" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="32" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="33" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="35" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="I19" s="34"/>
     </row>

</xml_diff>

<commit_message>
20210903 0017 tlw87 EOD updates.
</commit_message>
<xml_diff>
--- a/docs/AMT.xlsx
+++ b/docs/AMT.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw8748253\Desktop\Projects\Aromatic-Mountain-Technologies-BE\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Aromatic-Mountain-Technologies-BE\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3777B5D5-4FD6-4B8A-A482-4D734140EE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="470" yWindow="5070" windowWidth="27470" windowHeight="9990"/>
+    <workbookView xWindow="465" yWindow="3000" windowWidth="27465" windowHeight="12060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
     <sheet name="Postman" sheetId="2" r:id="rId2"/>
     <sheet name="RTM" sheetId="3" r:id="rId3"/>
+    <sheet name="States" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="274">
   <si>
     <t>Test Class</t>
   </si>
@@ -80,9 +91,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>/ers_login</t>
   </si>
   <si>
     <t>http://localhost:3015/ers_login</t>
@@ -494,16 +502,407 @@
   <si>
     <t>Test Number</t>
   </si>
+  <si>
+    <t>Get User by Username SUCCESS</t>
+  </si>
+  <si>
+    <t>/amt_user/:username</t>
+  </si>
+  <si>
+    <t>/tw8253</t>
+  </si>
+  <si>
+    <t>/amt_login</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_user/:username</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_user/tw8253</t>
+  </si>
+  <si>
+    <t>Add Customer SUCCESS</t>
+  </si>
+  <si>
+    <t>/amt_customer</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_customer</t>
+  </si>
+  <si>
+    <t>{
+	"username" : "tz1234",
+	"password" : "A_Pass1234",
+	"firstName" : "Tomas",
+	"lastName" : "Zecker",
+	"email" : "tomas.zecker@gmail.com"
+}</t>
+  </si>
+  <si>
+    <t>Add Address SUCCESS</t>
+  </si>
+  <si>
+    <t>/amt_adx/:username</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_adx/tz1234</t>
+  </si>
+  <si>
+    <t>ALABAMA</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>ALASKA</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AMERICAN SAMOA</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>ARIZONA</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>ARKANSAS</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>CALIFORNIA</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>COLORADO</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CONNECTICUT</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DELAWARE</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DISTRICT OF COLUMBIA</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>GUAM</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>HAWAII</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>IDAHO</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ILLINOIS</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>INDIANA</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>IOWA</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>KANSAS</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KENTUCKY</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LOUISIANA</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>MAINE</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MARYLAND</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MASSACHUSETTS</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MICHIGAN</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MINNESOTA</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MISSOURI</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MONTANA</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NEBRASKA</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NEVADA</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NEW HAMPSHIRE</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NEW JERSEY</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NEW MEXICO</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NORTH DAKOTA</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>NORTHERN MARIANA IS</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>OHIO</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OKLAHOMA</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OREGON</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PENNSYLVANIA</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PUERTO RICO</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>RHODE ISLAND</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SOUTH CAROLINA</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SOUTH DAKOTA</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>TENNESSEE</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UTAH</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>VERMONT</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>VIRGINIA</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VIRGIN ISLANDS</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>WASHINGTON</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WEST VIRGINIA</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WISCONSIN</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WYOMING</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>{
+	"addressLine1" : "5380 J St.",
+	"addressLine2" : "",
+	"addressCity" : "Penrose",
+	"addressState" : "CO",
+    "addressZipCode" : "81240",
+    "addressType" : "SHIPPING"
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000.00"/>
     <numFmt numFmtId="165" formatCode="000.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,8 +960,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF212121"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,8 +1003,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -623,11 +1033,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD7E1E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -721,6 +1161,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1001,35 +1447,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="83.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="141.26953125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="141.28515625" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1044,816 +1490,816 @@
         <v>4</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="28">
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>73</v>
-      </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="28">
         <v>1E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <f t="shared" ref="A4:A31" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="28">
         <v>2E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="28">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="28">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="28">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" t="s">
         <v>85</v>
       </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" t="s">
-        <v>86</v>
-      </c>
       <c r="H7" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="37">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="28">
         <v>1.0009999999999999</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="37">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="28">
         <v>1.002</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="28">
         <v>1.0029999999999999</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="37">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="28">
         <v>1.004</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="37">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="28">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="37">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="28">
         <v>2.0009999999999999</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="28">
         <v>2.0019999999999998</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" t="s">
         <v>104</v>
       </c>
-      <c r="G14" t="s">
-        <v>105</v>
-      </c>
       <c r="H14" s="25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="37">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="28">
         <v>2.0030000000000001</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" t="s">
         <v>104</v>
       </c>
-      <c r="G15" t="s">
-        <v>105</v>
-      </c>
       <c r="H15" s="25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="37">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="28">
         <v>2.004</v>
       </c>
       <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
         <v>103</v>
       </c>
-      <c r="E16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>104</v>
       </c>
-      <c r="G16" t="s">
-        <v>105</v>
-      </c>
       <c r="H16" s="25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="37">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="28">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="G17" t="s">
-        <v>86</v>
-      </c>
-      <c r="H17" s="25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="37">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="28">
         <v>3.0009999999999999</v>
       </c>
       <c r="D18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="37">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="28">
         <v>3.0019999999999998</v>
       </c>
       <c r="D19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G19" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="H19" s="25" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="37">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="28">
         <v>3.0030000000000001</v>
       </c>
       <c r="D20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="37">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="28">
         <v>3.004</v>
       </c>
       <c r="D21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
         <v>115</v>
       </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" t="s">
-        <v>116</v>
-      </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="37">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="28">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F22" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="G22" t="s">
-        <v>86</v>
-      </c>
-      <c r="H22" s="25" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="37">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="28">
         <v>4.0010000000000003</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="37">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="28">
         <v>4.0019999999999998</v>
       </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="37">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="28">
         <v>4.0030000000000001</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="37">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="28">
         <v>4.0039999999999996</v>
       </c>
       <c r="D26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
         <v>127</v>
       </c>
-      <c r="E26" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" t="s">
-        <v>128</v>
-      </c>
       <c r="G26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="37">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="28">
         <v>5</v>
       </c>
       <c r="D27" t="s">
+        <v>134</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
         <v>135</v>
       </c>
-      <c r="E27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" t="s">
-        <v>136</v>
-      </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="37">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="28">
         <v>5.0010000000000003</v>
       </c>
       <c r="D28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="37">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="28">
         <v>5.0019999999999998</v>
       </c>
       <c r="D29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G29" t="s">
+        <v>142</v>
+      </c>
+      <c r="H29" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="H29" s="25" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="37">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C30" s="28">
         <v>5.0030000000000001</v>
       </c>
       <c r="D30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="37">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="28">
         <v>5.0039999999999996</v>
       </c>
       <c r="D31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1863,31 +2309,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="4"/>
+    <col min="4" max="4" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -1916,7 +2362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -1924,26 +2370,26 @@
         <v>8</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>19</v>
-      </c>
       <c r="F2" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -1951,26 +2397,26 @@
         <v>8</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>19</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>20</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>8</v>
@@ -1983,7 +2429,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>8</v>
@@ -1996,20 +2442,32 @@
       <c r="H5" s="18"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>10</v>
+      </c>
       <c r="B6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18"/>
+      <c r="C6" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>150</v>
+      </c>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I6" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
         <v>8</v>
@@ -2022,10 +2480,8 @@
       <c r="H7" s="18"/>
       <c r="I7" s="23"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
-        <v>6</v>
-      </c>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
@@ -2037,10 +2493,8 @@
       <c r="H8" s="18"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="10">
-        <v>10</v>
-      </c>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
@@ -2052,10 +2506,8 @@
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
-        <v>10.01</v>
-      </c>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
@@ -2067,10 +2519,8 @@
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="10">
-        <v>10.02</v>
-      </c>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
         <v>8</v>
       </c>
@@ -2082,10 +2532,8 @@
       <c r="H11" s="18"/>
       <c r="I11" s="21"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="10">
-        <v>10.029999999999999</v>
-      </c>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
@@ -2097,10 +2545,8 @@
       <c r="H12" s="18"/>
       <c r="I12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="10">
-        <v>15</v>
-      </c>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
@@ -2112,10 +2558,8 @@
       <c r="H13" s="18"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="10">
-        <v>15.01</v>
-      </c>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
@@ -2127,10 +2571,8 @@
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="10">
-        <v>15.02</v>
-      </c>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>8</v>
       </c>
@@ -2142,10 +2584,8 @@
       <c r="H15" s="18"/>
       <c r="I15" s="21"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="10">
-        <v>15.03</v>
-      </c>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
         <v>8</v>
       </c>
@@ -2157,10 +2597,8 @@
       <c r="H16" s="18"/>
       <c r="I16" s="21"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10">
-        <v>20</v>
-      </c>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>8</v>
       </c>
@@ -2172,10 +2610,8 @@
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10">
-        <v>20.010000000000002</v>
-      </c>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
         <v>8</v>
       </c>
@@ -2187,10 +2623,8 @@
       <c r="H18" s="18"/>
       <c r="I18" s="22"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="10">
-        <v>20.02</v>
-      </c>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
         <v>8</v>
       </c>
@@ -2202,10 +2636,8 @@
       <c r="H19" s="18"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="10">
-        <v>21</v>
-      </c>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
         <v>8</v>
       </c>
@@ -2217,10 +2649,8 @@
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="10">
-        <v>21.01</v>
-      </c>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
         <v>8</v>
       </c>
@@ -2232,10 +2662,8 @@
       <c r="H21" s="18"/>
       <c r="I21" s="21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="10">
-        <v>21.02</v>
-      </c>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
         <v>8</v>
       </c>
@@ -2247,10 +2675,8 @@
       <c r="H22" s="18"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="10">
-        <v>25</v>
-      </c>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
         <v>8</v>
       </c>
@@ -2262,10 +2688,8 @@
       <c r="H23" s="18"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="10">
-        <v>25.01</v>
-      </c>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
         <v>8</v>
       </c>
@@ -2277,10 +2701,8 @@
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="10">
-        <v>25.02</v>
-      </c>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
       <c r="B25" s="11" t="s">
         <v>8</v>
       </c>
@@ -2292,10 +2714,8 @@
       <c r="H25" s="18"/>
       <c r="I25" s="21"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="10">
-        <v>25.03</v>
-      </c>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
         <v>8</v>
       </c>
@@ -2307,10 +2727,8 @@
       <c r="H26" s="18"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="10">
-        <v>25.04</v>
-      </c>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
         <v>8</v>
       </c>
@@ -2322,40 +2740,54 @@
       <c r="H27" s="18"/>
       <c r="I27" s="21"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>0</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="18"/>
+      <c r="C28" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>157</v>
+      </c>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
-        <v>0.01</v>
+        <v>5</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="18"/>
+      <c r="C29" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>273</v>
+      </c>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="14">
-        <v>0.02</v>
-      </c>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
       <c r="B30" s="15" t="s">
         <v>12</v>
       </c>
@@ -2367,10 +2799,8 @@
       <c r="H30" s="18"/>
       <c r="I30" s="21"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="14">
-        <v>0.03</v>
-      </c>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
       <c r="B31" s="15" t="s">
         <v>12</v>
       </c>
@@ -2382,10 +2812,8 @@
       <c r="H31" s="18"/>
       <c r="I31" s="21"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="14">
-        <v>1</v>
-      </c>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32" s="15" t="s">
         <v>12</v>
       </c>
@@ -2397,10 +2825,8 @@
       <c r="H32" s="18"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="14">
-        <v>2</v>
-      </c>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
       <c r="B33" s="15" t="s">
         <v>12</v>
       </c>
@@ -2412,10 +2838,8 @@
       <c r="H33" s="18"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="14">
-        <v>5</v>
-      </c>
+    <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
       <c r="B34" s="15" t="s">
         <v>12</v>
       </c>
@@ -2427,10 +2851,8 @@
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="14">
-        <v>6</v>
-      </c>
+    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
       <c r="B35" s="15" t="s">
         <v>12</v>
       </c>
@@ -2442,10 +2864,8 @@
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="14">
-        <v>0</v>
-      </c>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
       <c r="B36" s="16" t="s">
         <v>13</v>
       </c>
@@ -2457,10 +2877,8 @@
       <c r="H36" s="18"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="14">
-        <v>5</v>
-      </c>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
       <c r="B37" s="16" t="s">
         <v>13</v>
       </c>
@@ -2472,10 +2890,8 @@
       <c r="H37" s="18"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="10">
-        <v>5.01</v>
-      </c>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
       <c r="B38" s="16" t="s">
         <v>13</v>
       </c>
@@ -2487,10 +2903,8 @@
       <c r="H38" s="18"/>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="10">
-        <v>0</v>
-      </c>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
       <c r="B39" s="17" t="s">
         <v>14</v>
       </c>
@@ -2502,10 +2916,8 @@
       <c r="H39" s="18"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="10">
-        <v>0</v>
-      </c>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
       <c r="B40" s="17" t="s">
         <v>14</v>
       </c>
@@ -2517,10 +2929,8 @@
       <c r="H40" s="18"/>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="10">
-        <v>5</v>
-      </c>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
       <c r="B41" s="17" t="s">
         <v>14</v>
       </c>
@@ -2532,10 +2942,8 @@
       <c r="H41" s="18"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="10">
-        <v>5</v>
-      </c>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
       <c r="B42" s="17" t="s">
         <v>14</v>
       </c>
@@ -2547,10 +2955,8 @@
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="10">
-        <v>5.01</v>
-      </c>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
       <c r="B43" s="17" t="s">
         <v>14</v>
       </c>
@@ -2562,7 +2968,7 @@
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="13"/>
       <c r="C44" s="12"/>
@@ -2573,7 +2979,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="13"/>
       <c r="C45" s="12"/>
@@ -2584,7 +2990,7 @@
       <c r="H45" s="12"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="13"/>
       <c r="C46" s="12"/>
@@ -2595,7 +3001,7 @@
       <c r="H46" s="12"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="13"/>
       <c r="C47" s="12"/>
@@ -2606,7 +3012,7 @@
       <c r="H47" s="12"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="13"/>
       <c r="C48" s="12"/>
@@ -2617,7 +3023,7 @@
       <c r="H48" s="12"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="13"/>
       <c r="C49" s="12"/>
@@ -2628,7 +3034,7 @@
       <c r="H49" s="12"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="13"/>
       <c r="C50" s="12"/>
@@ -2639,7 +3045,7 @@
       <c r="H50" s="12"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="13"/>
       <c r="C51" s="12"/>
@@ -2650,7 +3056,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="13"/>
       <c r="C52" s="12"/>
@@ -2661,7 +3067,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="13"/>
       <c r="C53" s="12"/>
@@ -2672,7 +3078,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="13"/>
       <c r="C54" s="12"/>
@@ -2683,7 +3089,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="13"/>
       <c r="C55" s="12"/>
@@ -2694,7 +3100,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="13"/>
       <c r="C56" s="12"/>
@@ -2705,7 +3111,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="13"/>
       <c r="C57" s="12"/>
@@ -2716,7 +3122,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="13"/>
       <c r="C58" s="12"/>
@@ -2727,7 +3133,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="13"/>
       <c r="C59" s="12"/>
@@ -2738,7 +3144,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="13"/>
       <c r="C60" s="12"/>
@@ -2749,7 +3155,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
@@ -2760,7 +3166,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
@@ -2771,7 +3177,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
@@ -2782,7 +3188,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
@@ -2793,7 +3199,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
@@ -2804,7 +3210,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
@@ -2822,7 +3228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2830,420 +3236,420 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="75.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7265625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="35.453125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" style="29" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="30" t="s">
-        <v>33</v>
-      </c>
       <c r="E1" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="30" t="s">
-        <v>43</v>
-      </c>
       <c r="G1" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>56</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>57</v>
       </c>
       <c r="I1" s="31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
       <c r="G2" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I2" s="34"/>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
       <c r="G3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="I3" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
       <c r="G4" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="34" t="s">
-        <v>62</v>
-      </c>
       <c r="I4" s="34"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
       <c r="G5" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="34" t="s">
-        <v>62</v>
-      </c>
       <c r="I5" s="34"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="32"/>
       <c r="G6" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" s="34"/>
     </row>
-    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
       <c r="G7" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="35" t="s">
-        <v>64</v>
-      </c>
       <c r="I7" s="34"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I9" s="34"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I10" s="34"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="32"/>
       <c r="E11" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
       <c r="F12" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="32"/>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="D14" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="34"/>
       <c r="I14" s="34"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="32"/>
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="32"/>
       <c r="E18" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="34"/>
       <c r="I18" s="34"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I19" s="34"/>
     </row>
@@ -3251,4 +3657,471 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB116D3-935E-42F5-A0E3-8E423C75A72E}">
+  <dimension ref="A1:B56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="38" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="38" t="s">
+        <v>209</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="B28" s="38" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="B39" s="38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="B40" s="38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="B41" s="38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="B42" s="38" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="B43" s="38" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="B44" s="38" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="B45" s="38" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B48" s="38" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" s="38" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="B50" s="38" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="38" t="s">
+        <v>261</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="B53" s="38" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="B54" s="38" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="B56" s="39" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
20210903 1659 tlw8748253: EOD updates.
</commit_message>
<xml_diff>
--- a/docs/AMT.xlsx
+++ b/docs/AMT.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="287">
   <si>
     <t>Test Class</t>
   </si>
@@ -90,15 +90,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>http://localhost:3015/ers_login</t>
-  </si>
-  <si>
-    <t>?username=tlw874&amp;password=123456</t>
-  </si>
-  <si>
-    <t>User not validated</t>
   </si>
   <si>
     <t>ERSAdminService</t>
@@ -848,9 +839,6 @@
 }</t>
   </si>
   <si>
-    <t>Get current user request.</t>
-  </si>
-  <si>
     <t>Validate login session: VALID</t>
   </si>
   <si>
@@ -870,11 +858,56 @@
   </si>
   <si>
     <t>http://localhost:3025/amt_logout</t>
+  </si>
+  <si>
+    <t>/amt_phone/:username</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_phone/tz1234</t>
+  </si>
+  <si>
+    <t>{
+    "username": "ap1234",
+    "password": "A_Pass12345"
+}</t>
+  </si>
+  <si>
+    <t>Antonio Pierre</t>
+  </si>
+  <si>
+    <t>{
+    "username": "mr1234",
+    "password": "A_Pass12345"
+}</t>
+  </si>
+  <si>
+    <t>Matthew Rho</t>
+  </si>
+  <si>
+    <t>Add Catalog ItemSUCCESS</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_catalog_item</t>
+  </si>
+  <si>
+    <t>/amt_catalog_item</t>
+  </si>
+  <si>
+    <t>Add Phone Number SUCCESS</t>
   </si>
   <si>
     <t>{
     "loginUsername" : "tw8253",
     "loginPassword" : "A_Pass12345",
+ "catalogItem" : "French Roast",
+ "catalogItemDescription" : "French is the name applied to a degree of roast of coffee beans resulting in a dark brown coffee bean. In this roast, the beans are well into the second crack. French roasted beans will have a dark brown color and a shiney surface from its oils.",
+ "catalogItemPrice" : 12.95,
+ "catalogItemInStockQty" : 10,
+ "catalogItemType" : "BEANS"
+}</t>
+  </si>
+  <si>
+    <t>{
  "username" : "tz12345",
  "password" : "A_Pass1234",
  "firstName" : "Tomas",
@@ -884,8 +917,6 @@
   </si>
   <si>
     <t>{
-    "loginUsername" : "tw8253",
-    "loginPassword" : "A_Pass12345",
  "addressLine1" : "5380 J St.",
  "addressLine2" : "",
  "addressCity" : "Penrose",
@@ -895,31 +926,10 @@
 }</t>
   </si>
   <si>
-    <t>Add Phone Number SUCCESS Copy</t>
-  </si>
-  <si>
-    <t>/amt_phone/:username</t>
-  </si>
-  <si>
-    <t>http://localhost:3025/amt_phone/tz1234</t>
-  </si>
-  <si>
     <t>{
-    "username": "ap1234",
-    "password": "A_Pass12345"
+ "phoneNumber" : "7195551234",
+ "phoneNumberType" : "MOBILE"
 }</t>
-  </si>
-  <si>
-    <t>Antonio Pierre</t>
-  </si>
-  <si>
-    <t>{
-    "username": "mr1234",
-    "password": "A_Pass12345"
-}</t>
-  </si>
-  <si>
-    <t>Matthew Rho</t>
   </si>
 </sst>
 </file>
@@ -976,7 +986,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1016,6 +1026,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,7 +1093,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1174,6 +1190,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1476,13 +1495,13 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1497,7 +1516,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1505,25 +1524,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" s="27">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1532,25 +1551,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="27">
         <v>1E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1559,25 +1578,25 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C4" s="27">
         <v>2E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1586,25 +1605,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" s="27">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1613,25 +1632,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C6" s="27">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1640,25 +1659,25 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" s="27">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
         <v>79</v>
       </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>82</v>
-      </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1667,25 +1686,25 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="27">
         <v>1.0009999999999999</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1694,25 +1713,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C9" s="27">
         <v>1.002</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1721,25 +1740,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C10" s="27">
         <v>1.0029999999999999</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1748,25 +1767,25 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C11" s="27">
         <v>1.004</v>
       </c>
       <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" t="s">
         <v>86</v>
       </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" s="25" t="s">
         <v>89</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1775,25 +1794,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C12" s="27">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1802,25 +1821,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C13" s="27">
         <v>2.0009999999999999</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="25" t="s">
         <v>98</v>
-      </c>
-      <c r="G13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1829,25 +1848,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" s="27">
         <v>2.0019999999999998</v>
       </c>
       <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
         <v>95</v>
       </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>98</v>
-      </c>
       <c r="G14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>99</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1856,25 +1875,25 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C15" s="27">
         <v>2.0030000000000001</v>
       </c>
       <c r="D15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" t="s">
         <v>96</v>
       </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" t="s">
-        <v>99</v>
-      </c>
       <c r="H15" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1883,25 +1902,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="27">
         <v>2.004</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1910,25 +1929,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C17" s="27">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1937,25 +1956,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C18" s="27">
         <v>3.0009999999999999</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1964,25 +1983,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19" s="27">
         <v>3.0019999999999998</v>
       </c>
       <c r="D19" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
         <v>107</v>
       </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>110</v>
       </c>
-      <c r="G19" t="s">
-        <v>113</v>
-      </c>
       <c r="H19" s="25" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1991,25 +2010,25 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C20" s="27">
         <v>3.0030000000000001</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" t="s">
         <v>110</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" s="25" t="s">
         <v>113</v>
-      </c>
-      <c r="H20" s="25" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2018,25 +2037,25 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C21" s="27">
         <v>3.004</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" t="s">
         <v>110</v>
       </c>
-      <c r="G21" t="s">
-        <v>113</v>
-      </c>
       <c r="H21" s="25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2045,25 +2064,25 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C22" s="27">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2072,25 +2091,25 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C23" s="27">
         <v>4.0010000000000003</v>
       </c>
       <c r="D23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2099,25 +2118,25 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C24" s="27">
         <v>4.0019999999999998</v>
       </c>
       <c r="D24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" t="s">
         <v>119</v>
       </c>
-      <c r="E24" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="25" t="s">
         <v>122</v>
-      </c>
-      <c r="G24" t="s">
-        <v>128</v>
-      </c>
-      <c r="H24" s="25" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2126,25 +2145,25 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C25" s="27">
         <v>4.0030000000000001</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G25" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2153,25 +2172,25 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C26" s="27">
         <v>4.0039999999999996</v>
       </c>
       <c r="D26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2180,25 +2199,25 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C27" s="27">
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2207,25 +2226,25 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C28" s="27">
         <v>5.0010000000000003</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F28" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2234,25 +2253,25 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C29" s="27">
         <v>5.0019999999999998</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E29" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2261,25 +2280,25 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C30" s="27">
         <v>5.0030000000000001</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G30" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2288,25 +2307,25 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C31" s="27">
         <v>5.0039999999999996</v>
       </c>
       <c r="D31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>127</v>
+      </c>
+      <c r="G31" t="s">
         <v>134</v>
       </c>
-      <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" t="s">
-        <v>130</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="H31" s="25" t="s">
         <v>137</v>
-      </c>
-      <c r="H31" s="25" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2320,10 +2339,10 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -2331,7 +2350,7 @@
     <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
-    <col min="4" max="4" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.54296875" style="4" customWidth="1"/>
     <col min="6" max="6" width="37.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
@@ -2383,28 +2402,16 @@
       <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="10">
-        <v>5</v>
-      </c>
+      <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>19</v>
-      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="18" t="s">
-        <v>20</v>
-      </c>
+      <c r="H3" s="18"/>
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9">
@@ -2441,21 +2448,21 @@
         <v>8</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D6" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>147</v>
-      </c>
       <c r="F6" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G6" s="18"/>
       <c r="H6" s="18"/>
       <c r="I6" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2739,16 +2746,16 @@
         <v>12</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
@@ -2762,21 +2769,21 @@
         <v>12</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
       <c r="I29" s="19" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="58">
@@ -2787,21 +2794,21 @@
         <v>12</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
       <c r="I30" s="19" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1">
@@ -2838,16 +2845,16 @@
         <v>12</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D33" s="19" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
@@ -2861,22 +2868,22 @@
         <v>12</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" ht="130.5">
+    <row r="35" spans="1:9" ht="101.5">
       <c r="A35" s="10">
         <v>5</v>
       </c>
@@ -2884,22 +2891,22 @@
         <v>12</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D35" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" ht="145">
+    <row r="36" spans="1:9" ht="116">
       <c r="A36" s="14">
         <v>10</v>
       </c>
@@ -2907,22 +2914,22 @@
         <v>12</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
       <c r="I36" s="18"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" ht="58">
       <c r="A37" s="14">
         <v>12</v>
       </c>
@@ -2930,28 +2937,40 @@
         <v>12</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="F37" s="18"/>
+        <v>274</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>286</v>
+      </c>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
       <c r="I37" s="21"/>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="14"/>
+    <row r="38" spans="1:9" ht="217.5">
+      <c r="A38" s="14">
+        <v>15</v>
+      </c>
       <c r="B38" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="18"/>
+      <c r="C38" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="F38" s="39" t="s">
+        <v>283</v>
+      </c>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
       <c r="I38" s="21"/>
@@ -3394,28 +3413,28 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I1" s="30" t="s">
         <v>17</v>
@@ -3423,214 +3442,214 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
       <c r="G2" s="32" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="29">
       <c r="A3" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
       <c r="G3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="33" t="s">
-        <v>56</v>
-      </c>
       <c r="I3" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B4" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>28</v>
-      </c>
       <c r="D4" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
       <c r="G4" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I4" s="33"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
       <c r="G5" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
       <c r="G6" s="31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:9" ht="29">
       <c r="A7" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
       <c r="G7" s="31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H7" s="34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I7" s="33"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F8" s="31"/>
       <c r="G8" s="31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I8" s="33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
       <c r="H10" s="34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I10" s="33"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31"/>
       <c r="E11" s="32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
@@ -3639,16 +3658,16 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
       <c r="F12" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G12" s="31"/>
       <c r="H12" s="33"/>
@@ -3656,16 +3675,16 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
       <c r="F13" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G13" s="31"/>
       <c r="H13" s="33"/>
@@ -3673,20 +3692,20 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" s="31"/>
       <c r="F14" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G14" s="31"/>
       <c r="H14" s="33"/>
@@ -3694,20 +3713,20 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="31"/>
       <c r="F15" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G15" s="31"/>
       <c r="H15" s="33"/>
@@ -3715,20 +3734,20 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" s="31"/>
       <c r="F16" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="33"/>
@@ -3736,20 +3755,20 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G17" s="31"/>
       <c r="H17" s="33"/>
@@ -3757,18 +3776,18 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
       <c r="E18" s="32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G18" s="31"/>
       <c r="H18" s="33"/>
@@ -3776,24 +3795,24 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F19" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G19" s="31"/>
       <c r="H19" s="34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I19" s="33"/>
     </row>
@@ -3819,450 +3838,450 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" thickBot="1">
       <c r="A1" s="37" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" thickBot="1">
       <c r="A2" s="37" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" thickBot="1">
       <c r="A3" s="37" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" thickBot="1">
       <c r="A4" s="37" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" thickBot="1">
       <c r="A5" s="37" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" thickBot="1">
       <c r="A6" s="37" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" thickBot="1">
       <c r="A7" s="37" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" thickBot="1">
       <c r="A8" s="37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19.5" thickBot="1">
       <c r="A9" s="37" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" thickBot="1">
       <c r="A10" s="37" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" thickBot="1">
       <c r="A11" s="37" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" thickBot="1">
       <c r="A12" s="37" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" thickBot="1">
       <c r="A13" s="37" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" thickBot="1">
       <c r="A14" s="37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" thickBot="1">
       <c r="A15" s="37" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" thickBot="1">
       <c r="A16" s="37" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19.5" thickBot="1">
       <c r="A17" s="37" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19.5" thickBot="1">
       <c r="A18" s="37" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19.5" thickBot="1">
       <c r="A19" s="37" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19.5" thickBot="1">
       <c r="A20" s="37" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19.5" thickBot="1">
       <c r="A21" s="37" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19.5" thickBot="1">
       <c r="A22" s="37" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19.5" thickBot="1">
       <c r="A23" s="37" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19.5" thickBot="1">
       <c r="A24" s="37" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19.5" thickBot="1">
       <c r="A25" s="37" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19.5" thickBot="1">
       <c r="A26" s="37" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19.5" thickBot="1">
       <c r="A27" s="37" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="19.5" thickBot="1">
       <c r="A28" s="37" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19.5" thickBot="1">
       <c r="A29" s="37" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19.5" thickBot="1">
       <c r="A30" s="37" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19.5" thickBot="1">
       <c r="A31" s="37" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19.5" thickBot="1">
       <c r="A32" s="37" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19.5" thickBot="1">
       <c r="A33" s="37" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19.5" thickBot="1">
       <c r="A34" s="37" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19.5" thickBot="1">
       <c r="A35" s="37" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19.5" thickBot="1">
       <c r="A36" s="37" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19.5" thickBot="1">
       <c r="A37" s="37" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19.5" thickBot="1">
       <c r="A38" s="37" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19.5" thickBot="1">
       <c r="A39" s="37" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="19.5" thickBot="1">
       <c r="A40" s="37" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="19.5" thickBot="1">
       <c r="A41" s="37" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="19.5" thickBot="1">
       <c r="A42" s="37" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="19.5" thickBot="1">
       <c r="A43" s="37" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="19.5" thickBot="1">
       <c r="A44" s="37" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="19.5" thickBot="1">
       <c r="A45" s="37" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="19.5" thickBot="1">
       <c r="A46" s="37" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="19.5" thickBot="1">
       <c r="A47" s="37" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B47" s="37" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="19.5" thickBot="1">
       <c r="A48" s="37" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="19.5" thickBot="1">
       <c r="A49" s="37" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B49" s="37" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="19.5" thickBot="1">
       <c r="A50" s="37" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B50" s="37" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="19.5" thickBot="1">
       <c r="A51" s="37" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B51" s="37" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="19.5" thickBot="1">
       <c r="A52" s="37" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B52" s="37" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="19.5" thickBot="1">
       <c r="A53" s="37" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B53" s="37" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="19.5" thickBot="1">
       <c r="A54" s="37" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B54" s="37" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="19.5" thickBot="1">
       <c r="A55" s="37" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B55" s="37" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="19">
       <c r="A56" s="38" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20210905 1451 tlw87 code baseline 01 all add paths completed.
</commit_message>
<xml_diff>
--- a/docs/AMT.xlsx
+++ b/docs/AMT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw8748253\Desktop\Projects\Aromatic-Mountain-Technologies-BE\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Aromatic-Mountain-Technologies-BE\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D63B5B-B662-4F5B-839B-8A5D631CBAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="470" yWindow="3000" windowWidth="27470" windowHeight="12060" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="RTM" sheetId="3" r:id="rId3"/>
     <sheet name="States" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="292">
   <si>
     <t>Test Class</t>
   </si>
@@ -489,9 +490,6 @@
   </si>
   <si>
     <t>/amt_adx/:username</t>
-  </si>
-  <si>
-    <t>http://localhost:3025/amt_adx/tz1234</t>
   </si>
   <si>
     <t>ALABAMA</t>
@@ -861,9 +859,6 @@
   </si>
   <si>
     <t>/amt_phone/:username</t>
-  </si>
-  <si>
-    <t>http://localhost:3025/amt_phone/tz1234</t>
   </si>
   <si>
     <t>{
@@ -908,15 +903,6 @@
   </si>
   <si>
     <t>{
- "username" : "tz12345",
- "password" : "A_Pass1234",
- "firstName" : "Tomas",
- "lastName" : "Zecker",
- "email" : "tomas.zecker@gmail.com"
-}</t>
-  </si>
-  <si>
-    <t>{
  "addressLine1" : "5380 J St.",
  "addressLine2" : "",
  "addressCity" : "Penrose",
@@ -931,16 +917,60 @@
  "phoneNumberType" : "MOBILE"
 }</t>
   </si>
+  <si>
+    <t>Add Catalog Item INVALID employee role</t>
+  </si>
+  <si>
+    <t>Add Customer Order SUCCESS</t>
+  </si>
+  <si>
+    <t>/amt_order</t>
+  </si>
+  <si>
+    <t>{
+    "orderAmount" : "26.95",
+    "lstOrderedItem" : [
+	{
+		"catalogItemName" : "FRROAST0001",
+		"orderItemPrice" : 12.97,
+		"orderItemQty" : 1
+	},
+	{
+		"catalogItemName" : "FRVANILLA0001",
+		"orderItemPrice" : 5.95,
+		"orderItemQty" : 2
+	}
+	]
+}</t>
+  </si>
+  <si>
+    <t>{
+ "username" : "tz12346",
+ "password" : "A_Pass1234",
+ "firstName" : "Tomas",
+ "lastName" : "Zecker",
+ "email" : "tomas.zecker@gmail.com"
+}</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_adx/tz12346</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_phone/tz12346</t>
+  </si>
+  <si>
+    <t>http://localhost:3025/amt_order/tz12346</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="000.00"/>
     <numFmt numFmtId="165" formatCode="000.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1093,7 +1123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1150,10 +1180,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1193,6 +1219,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1473,7 +1502,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1481,26 +1510,26 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="83.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="141.26953125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="141.28515625" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="24" t="s">
         <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1515,18 +1544,18 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="22" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="36">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="25">
         <v>0</v>
       </c>
       <c r="D2" t="s">
@@ -1541,19 +1570,19 @@
       <c r="G2" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="36">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="25">
         <v>1E-3</v>
       </c>
       <c r="D3" t="s">
@@ -1568,19 +1597,19 @@
       <c r="G3" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="23" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="36">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
         <f t="shared" ref="A4:A31" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="25">
         <v>2E-3</v>
       </c>
       <c r="D4" t="s">
@@ -1595,19 +1624,19 @@
       <c r="G4" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="36">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="25">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D5" t="s">
@@ -1622,19 +1651,19 @@
       <c r="G5" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="36">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="34">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="25">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D6" t="s">
@@ -1649,19 +1678,19 @@
       <c r="G6" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="36">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="25">
         <v>1</v>
       </c>
       <c r="D7" t="s">
@@ -1676,19 +1705,19 @@
       <c r="G7" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="36">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="34">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="25">
         <v>1.0009999999999999</v>
       </c>
       <c r="D8" t="s">
@@ -1703,19 +1732,19 @@
       <c r="G8" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="23" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="36">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="25">
         <v>1.002</v>
       </c>
       <c r="D9" t="s">
@@ -1730,19 +1759,19 @@
       <c r="G9" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="23" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="36">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="25">
         <v>1.0029999999999999</v>
       </c>
       <c r="D10" t="s">
@@ -1757,19 +1786,19 @@
       <c r="G10" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="36">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="34">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="25">
         <v>1.004</v>
       </c>
       <c r="D11" t="s">
@@ -1784,19 +1813,19 @@
       <c r="G11" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="36">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="34">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="25">
         <v>2</v>
       </c>
       <c r="D12" t="s">
@@ -1811,19 +1840,19 @@
       <c r="G12" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="36">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="25">
         <v>2.0009999999999999</v>
       </c>
       <c r="D13" t="s">
@@ -1838,19 +1867,19 @@
       <c r="G13" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="36">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="25">
         <v>2.0019999999999998</v>
       </c>
       <c r="D14" t="s">
@@ -1865,19 +1894,19 @@
       <c r="G14" t="s">
         <v>96</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="36">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="25">
         <v>2.0030000000000001</v>
       </c>
       <c r="D15" t="s">
@@ -1892,19 +1921,19 @@
       <c r="G15" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="23" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="36">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="34">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="25">
         <v>2.004</v>
       </c>
       <c r="D16" t="s">
@@ -1919,19 +1948,19 @@
       <c r="G16" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="23" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="36">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="34">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="25">
         <v>3</v>
       </c>
       <c r="D17" t="s">
@@ -1946,19 +1975,19 @@
       <c r="G17" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="36">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="34">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="25">
         <v>3.0009999999999999</v>
       </c>
       <c r="D18" t="s">
@@ -1973,19 +2002,19 @@
       <c r="G18" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="36">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="34">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="25">
         <v>3.0019999999999998</v>
       </c>
       <c r="D19" t="s">
@@ -2000,19 +2029,19 @@
       <c r="G19" t="s">
         <v>110</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="23" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="36">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="34">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="25">
         <v>3.0030000000000001</v>
       </c>
       <c r="D20" t="s">
@@ -2027,19 +2056,19 @@
       <c r="G20" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="23" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="36">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="34">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="25">
         <v>3.004</v>
       </c>
       <c r="D21" t="s">
@@ -2054,19 +2083,19 @@
       <c r="G21" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="23" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="36">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="34">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="25">
         <v>4</v>
       </c>
       <c r="D22" t="s">
@@ -2081,19 +2110,19 @@
       <c r="G22" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="23" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="36">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="34">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="25">
         <v>4.0010000000000003</v>
       </c>
       <c r="D23" t="s">
@@ -2108,19 +2137,19 @@
       <c r="G23" t="s">
         <v>78</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="23" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="36">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="34">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C24" s="25">
         <v>4.0019999999999998</v>
       </c>
       <c r="D24" t="s">
@@ -2135,19 +2164,19 @@
       <c r="G24" t="s">
         <v>125</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="36">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="34">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="27">
+      <c r="C25" s="25">
         <v>4.0030000000000001</v>
       </c>
       <c r="D25" t="s">
@@ -2162,19 +2191,19 @@
       <c r="G25" t="s">
         <v>125</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="23" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="36">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="34">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C26" s="25">
         <v>4.0039999999999996</v>
       </c>
       <c r="D26" t="s">
@@ -2189,19 +2218,19 @@
       <c r="G26" t="s">
         <v>125</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="23" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="36">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="34">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="25">
         <v>5</v>
       </c>
       <c r="D27" t="s">
@@ -2216,19 +2245,19 @@
       <c r="G27" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="25" t="s">
+      <c r="H27" s="23" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="36">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="34">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C28" s="25">
         <v>5.0010000000000003</v>
       </c>
       <c r="D28" t="s">
@@ -2243,19 +2272,19 @@
       <c r="G28" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="25" t="s">
+      <c r="H28" s="23" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="36">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="34">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="25">
         <v>5.0019999999999998</v>
       </c>
       <c r="D29" t="s">
@@ -2270,19 +2299,19 @@
       <c r="G29" t="s">
         <v>134</v>
       </c>
-      <c r="H29" s="25" t="s">
+      <c r="H29" s="23" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="36">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="34">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="27">
+      <c r="C30" s="25">
         <v>5.0030000000000001</v>
       </c>
       <c r="D30" t="s">
@@ -2297,19 +2326,19 @@
       <c r="G30" t="s">
         <v>134</v>
       </c>
-      <c r="H30" s="25" t="s">
+      <c r="H30" s="23" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="36">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="34">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="25">
         <v>5.0039999999999996</v>
       </c>
       <c r="D31" t="s">
@@ -2324,7 +2353,7 @@
       <c r="G31" t="s">
         <v>134</v>
       </c>
-      <c r="H31" s="25" t="s">
+      <c r="H31" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2335,31 +2364,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.54296875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="37.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="4"/>
+    <col min="4" max="4" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -2388,7 +2417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>8</v>
@@ -2401,7 +2430,7 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
         <v>8</v>
@@ -2414,7 +2443,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="19"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
         <v>8</v>
@@ -2427,7 +2456,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="19"/>
     </row>
-    <row r="5" spans="1:9" hidden="1">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
         <v>8</v>
@@ -2440,7 +2469,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="19"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>10</v>
       </c>
@@ -2465,7 +2494,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="11" t="s">
         <v>8</v>
@@ -2476,9 +2505,9 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="I7" s="21"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11" t="s">
         <v>8</v>
@@ -2491,254 +2520,254 @@
       <c r="H8" s="18"/>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
       <c r="H10" s="18"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
-      <c r="I11" s="21"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="I11" s="38"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
-      <c r="I12" s="21"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="I12" s="38"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
       <c r="I13" s="19"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
-      <c r="I15" s="21"/>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="I15" s="38"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
-      <c r="I16" s="21"/>
-    </row>
-    <row r="17" spans="1:9" hidden="1">
+      <c r="I16" s="38"/>
+    </row>
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" hidden="1">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
-      <c r="I18" s="22"/>
-    </row>
-    <row r="19" spans="1:9" hidden="1">
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
-      <c r="I19" s="21"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="I19" s="38"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="21"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="I21" s="38"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
-      <c r="I22" s="21"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="I22" s="38"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
-      <c r="I25" s="21"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="I25" s="38"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
-      <c r="I26" s="21"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="I26" s="38"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
-      <c r="I27" s="21"/>
-    </row>
-    <row r="28" spans="1:9" ht="58">
+      <c r="I27" s="38"/>
+    </row>
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>2</v>
       </c>
@@ -2746,22 +2775,22 @@
         <v>12</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>143</v>
       </c>
       <c r="E28" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>264</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>265</v>
       </c>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
-      <c r="I28" s="21"/>
-    </row>
-    <row r="29" spans="1:9" ht="58">
+      <c r="I28" s="38"/>
+    </row>
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>2.0099999999999998</v>
       </c>
@@ -2769,24 +2798,24 @@
         <v>12</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>143</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
       <c r="I29" s="19" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="58">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>2.02</v>
       </c>
@@ -2794,50 +2823,50 @@
         <v>12</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>143</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
       <c r="I30" s="19" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="6" customFormat="1">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="19"/>
-      <c r="E31" s="20"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="19"/>
-      <c r="E32" s="20"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
-      <c r="I32" s="21"/>
-    </row>
-    <row r="33" spans="1:9" ht="58">
+      <c r="I32" s="38"/>
+    </row>
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>3</v>
       </c>
@@ -2845,22 +2874,22 @@
         <v>12</v>
       </c>
       <c r="C33" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="E33" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="E33" s="19" t="s">
-        <v>268</v>
-      </c>
       <c r="F33" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" ht="58">
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>4</v>
       </c>
@@ -2868,22 +2897,22 @@
         <v>12</v>
       </c>
       <c r="C34" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="E34" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="E34" s="19" t="s">
-        <v>272</v>
-      </c>
       <c r="F34" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" ht="101.5">
+    <row r="35" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>5</v>
       </c>
@@ -2900,13 +2929,13 @@
         <v>148</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="G35" s="18"/>
       <c r="H35" s="18"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" ht="116">
+    <row r="36" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>10</v>
       </c>
@@ -2920,16 +2949,16 @@
         <v>150</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>151</v>
+        <v>289</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
       <c r="I36" s="18"/>
     </row>
-    <row r="37" spans="1:9" ht="58">
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>12</v>
       </c>
@@ -2937,22 +2966,22 @@
         <v>12</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
-      <c r="I37" s="21"/>
-    </row>
-    <row r="38" spans="1:9" ht="217.5">
+      <c r="I37" s="38"/>
+    </row>
+    <row r="38" spans="1:9" ht="225" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>15</v>
       </c>
@@ -2960,74 +2989,92 @@
         <v>12</v>
       </c>
       <c r="C38" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="D38" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="E38" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="F38" s="37" t="s">
         <v>281</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="F38" s="39" t="s">
-        <v>283</v>
       </c>
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
-      <c r="I38" s="21"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="14"/>
+      <c r="I38" s="38"/>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
+        <v>15.01</v>
+      </c>
       <c r="B39" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="20"/>
+      <c r="C39" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>278</v>
+      </c>
       <c r="F39" s="18"/>
       <c r="G39" s="18"/>
       <c r="H39" s="18"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="14"/>
+    <row r="40" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>20</v>
+      </c>
       <c r="B40" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="18"/>
+      <c r="C40" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>287</v>
+      </c>
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" s="6" customFormat="1">
+    <row r="41" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="19"/>
-      <c r="E41" s="20"/>
+      <c r="E41" s="19"/>
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
       <c r="I41" s="18"/>
     </row>
-    <row r="42" spans="1:9" s="6" customFormat="1">
+    <row r="42" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
       <c r="B42" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="19"/>
-      <c r="E42" s="20"/>
+      <c r="E42" s="19"/>
       <c r="F42" s="18"/>
       <c r="G42" s="18"/>
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="16" t="s">
         <v>13</v>
@@ -3040,20 +3087,20 @@
       <c r="H43" s="18"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="19"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="19"/>
       <c r="F44" s="18"/>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="16" t="s">
         <v>13</v>
@@ -3066,7 +3113,7 @@
       <c r="H45" s="18"/>
       <c r="I45" s="18"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="17" t="s">
         <v>14</v>
@@ -3079,7 +3126,7 @@
       <c r="H46" s="18"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="17" t="s">
         <v>14</v>
@@ -3092,7 +3139,7 @@
       <c r="H47" s="18"/>
       <c r="I47" s="18"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="17" t="s">
         <v>14</v>
@@ -3105,7 +3152,7 @@
       <c r="H48" s="18"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="17" t="s">
         <v>14</v>
@@ -3118,7 +3165,7 @@
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="10"/>
       <c r="B50" s="17" t="s">
         <v>14</v>
@@ -3131,7 +3178,7 @@
       <c r="H50" s="18"/>
       <c r="I50" s="19"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="13"/>
       <c r="C51" s="12"/>
@@ -3142,7 +3189,7 @@
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="10"/>
       <c r="B52" s="13"/>
       <c r="C52" s="12"/>
@@ -3153,7 +3200,7 @@
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
       <c r="B53" s="13"/>
       <c r="C53" s="12"/>
@@ -3164,7 +3211,7 @@
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="13"/>
       <c r="C54" s="12"/>
@@ -3175,7 +3222,7 @@
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="10"/>
       <c r="B55" s="13"/>
       <c r="C55" s="12"/>
@@ -3186,7 +3233,7 @@
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="13"/>
       <c r="C56" s="12"/>
@@ -3197,7 +3244,7 @@
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="10"/>
       <c r="B57" s="13"/>
       <c r="C57" s="12"/>
@@ -3208,7 +3255,7 @@
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
       <c r="B58" s="13"/>
       <c r="C58" s="12"/>
@@ -3219,7 +3266,7 @@
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="13"/>
       <c r="C59" s="12"/>
@@ -3230,7 +3277,7 @@
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="13"/>
       <c r="C60" s="12"/>
@@ -3241,7 +3288,7 @@
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="13"/>
       <c r="C61" s="12"/>
@@ -3252,7 +3299,7 @@
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="13"/>
       <c r="C62" s="12"/>
@@ -3263,7 +3310,7 @@
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="13"/>
       <c r="C63" s="12"/>
@@ -3274,7 +3321,7 @@
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="13"/>
       <c r="C64" s="12"/>
@@ -3285,7 +3332,7 @@
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="13"/>
       <c r="C65" s="12"/>
@@ -3296,7 +3343,7 @@
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="13"/>
       <c r="C66" s="12"/>
@@ -3307,7 +3354,7 @@
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="13"/>
       <c r="C67" s="12"/>
@@ -3318,7 +3365,7 @@
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="13"/>
       <c r="C68" s="12"/>
@@ -3329,7 +3376,7 @@
       <c r="H68" s="12"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="13"/>
       <c r="C69" s="12"/>
@@ -3340,7 +3387,7 @@
       <c r="H69" s="12"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="13"/>
       <c r="C70" s="12"/>
@@ -3351,7 +3398,7 @@
       <c r="H70" s="12"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="13"/>
       <c r="C71" s="12"/>
@@ -3362,7 +3409,7 @@
       <c r="H71" s="12"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="13"/>
       <c r="C72" s="12"/>
@@ -3373,7 +3420,7 @@
       <c r="H72" s="12"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="13"/>
       <c r="C73" s="12"/>
@@ -3391,7 +3438,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3399,422 +3446,422 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="75.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7265625" style="28" customWidth="1"/>
-    <col min="9" max="9" width="35.453125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" style="26" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="28" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32" t="s">
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="33"/>
-    </row>
-    <row r="3" spans="1:9" ht="29">
-      <c r="A3" s="31" t="s">
+      <c r="I2" s="31"/>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32" t="s">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="33"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="31" t="s">
+      <c r="I4" s="31"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="32" t="s">
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="33"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="31" t="s">
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="1:9" ht="29">
-      <c r="A7" s="31" t="s">
+      <c r="I6" s="31"/>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32" t="s">
+      <c r="C7" s="29"/>
+      <c r="D7" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31" t="s">
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="33"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="31" t="s">
+      <c r="I7" s="31"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31" t="s">
+      <c r="F8" s="29"/>
+      <c r="G8" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32" t="s">
+      <c r="C9" s="29"/>
+      <c r="D9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="34" t="s">
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="33"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="31" t="s">
+      <c r="I9" s="31"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="32" t="s">
+      <c r="C10" s="29"/>
+      <c r="D10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="34" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="33"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="31" t="s">
+      <c r="I10" s="31"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32" t="s">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="31" t="s">
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="31" t="s">
+      <c r="G12" s="29"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32" t="s">
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="31" t="s">
+      <c r="G13" s="29"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32" t="s">
+      <c r="E14" s="29"/>
+      <c r="F14" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="31" t="s">
+      <c r="G14" s="29"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32" t="s">
+      <c r="E15" s="29"/>
+      <c r="F15" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="31" t="s">
+      <c r="G15" s="29"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32" t="s">
+      <c r="E16" s="29"/>
+      <c r="F16" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="31" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32" t="s">
+      <c r="E17" s="29"/>
+      <c r="F17" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="31" t="s">
+      <c r="G17" s="29"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32" t="s">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="31" t="s">
+      <c r="G18" s="29"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32" t="s">
+      <c r="C19" s="29"/>
+      <c r="D19" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="34" t="s">
+      <c r="G19" s="29"/>
+      <c r="H19" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="33"/>
+      <c r="I19" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3823,465 +3870,465 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="B1" s="37" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A2" s="37" t="s">
+      <c r="B2" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="37" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A3" s="37" t="s">
+      <c r="B3" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="37" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A4" s="37" t="s">
+      <c r="B4" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="B4" s="37" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A5" s="37" t="s">
+      <c r="B5" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="B5" s="37" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A6" s="37" t="s">
+      <c r="B6" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="37" t="s">
+    </row>
+    <row r="7" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A7" s="37" t="s">
+      <c r="B7" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="B7" s="37" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="B8" s="37" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="35" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A9" s="37" t="s">
+      <c r="B9" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="B9" s="37" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A10" s="37" t="s">
+      <c r="B10" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="B10" s="37" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A11" s="37" t="s">
+      <c r="B11" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="B11" s="37" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="35" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A12" s="37" t="s">
+      <c r="B12" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="37" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="35" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A13" s="37" t="s">
+      <c r="B13" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="B13" s="37" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A14" s="37" t="s">
+      <c r="B14" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="B14" s="37" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A15" s="37" t="s">
+      <c r="B15" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="B15" s="37" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="35" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A16" s="37" t="s">
+      <c r="B16" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="B16" s="37" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A17" s="37" t="s">
+      <c r="B17" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="B17" s="37" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A18" s="37" t="s">
+      <c r="B18" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="B18" s="37" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A19" s="37" t="s">
+      <c r="B19" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="B19" s="37" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A20" s="37" t="s">
+      <c r="B20" s="35" t="s">
         <v>190</v>
       </c>
-      <c r="B20" s="37" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="35" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A21" s="37" t="s">
+      <c r="B21" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="B21" s="37" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A22" s="37" t="s">
+      <c r="B22" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="B22" s="37" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A23" s="37" t="s">
+      <c r="B23" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="B23" s="37" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="35" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A24" s="37" t="s">
+      <c r="B24" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="B24" s="37" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A25" s="37" t="s">
+      <c r="B25" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="37" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="35" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A26" s="37" t="s">
+      <c r="B26" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="B26" s="37" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="35" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A27" s="37" t="s">
+      <c r="B27" s="35" t="s">
         <v>204</v>
       </c>
-      <c r="B27" s="37" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="35" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A28" s="37" t="s">
+      <c r="B28" s="35" t="s">
         <v>206</v>
       </c>
-      <c r="B28" s="37" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="35" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A29" s="37" t="s">
+      <c r="B29" s="35" t="s">
         <v>208</v>
       </c>
-      <c r="B29" s="37" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="35" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A30" s="37" t="s">
+      <c r="B30" s="35" t="s">
         <v>210</v>
       </c>
-      <c r="B30" s="37" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="35" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A31" s="37" t="s">
+      <c r="B31" s="35" t="s">
         <v>212</v>
       </c>
-      <c r="B31" s="37" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="35" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A32" s="37" t="s">
+      <c r="B32" s="35" t="s">
         <v>214</v>
       </c>
-      <c r="B32" s="37" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="35" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A33" s="37" t="s">
+      <c r="B33" s="35" t="s">
         <v>216</v>
       </c>
-      <c r="B33" s="37" t="s">
+    </row>
+    <row r="34" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="35" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A34" s="37" t="s">
+      <c r="B34" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="B34" s="37" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="35" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A35" s="37" t="s">
+      <c r="B35" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="B35" s="37" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="35" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A36" s="37" t="s">
+      <c r="B36" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="B36" s="37" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="35" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A37" s="37" t="s">
+      <c r="B37" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="B37" s="37" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="35" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A38" s="37" t="s">
+      <c r="B38" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="B38" s="37" t="s">
+    </row>
+    <row r="39" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="35" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A39" s="37" t="s">
+      <c r="B39" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="B39" s="37" t="s">
+    </row>
+    <row r="40" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="35" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A40" s="37" t="s">
+      <c r="B40" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="B40" s="37" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="35" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A41" s="37" t="s">
+      <c r="B41" s="35" t="s">
         <v>232</v>
       </c>
-      <c r="B41" s="37" t="s">
+    </row>
+    <row r="42" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="35" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A42" s="37" t="s">
+      <c r="B42" s="35" t="s">
         <v>234</v>
       </c>
-      <c r="B42" s="37" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="35" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A43" s="37" t="s">
+      <c r="B43" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="B43" s="37" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="35" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A44" s="37" t="s">
+      <c r="B44" s="35" t="s">
         <v>238</v>
       </c>
-      <c r="B44" s="37" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="35" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A45" s="37" t="s">
+      <c r="B45" s="35" t="s">
         <v>240</v>
       </c>
-      <c r="B45" s="37" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="35" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A46" s="37" t="s">
+      <c r="B46" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="B46" s="37" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="35" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A47" s="37" t="s">
+      <c r="B47" s="35" t="s">
         <v>244</v>
       </c>
-      <c r="B47" s="37" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="35" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A48" s="37" t="s">
+      <c r="B48" s="35" t="s">
         <v>246</v>
       </c>
-      <c r="B48" s="37" t="s">
+    </row>
+    <row r="49" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="35" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A49" s="37" t="s">
+      <c r="B49" s="35" t="s">
         <v>248</v>
       </c>
-      <c r="B49" s="37" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="35" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A50" s="37" t="s">
+      <c r="B50" s="35" t="s">
         <v>250</v>
       </c>
-      <c r="B50" s="37" t="s">
+    </row>
+    <row r="51" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="35" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A51" s="37" t="s">
+      <c r="B51" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="B51" s="37" t="s">
+    </row>
+    <row r="52" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="35" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A52" s="37" t="s">
+      <c r="B52" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="B52" s="37" t="s">
+    </row>
+    <row r="53" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="35" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A53" s="37" t="s">
+      <c r="B53" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="B53" s="37" t="s">
+    </row>
+    <row r="54" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="35" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A54" s="37" t="s">
+      <c r="B54" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="B54" s="37" t="s">
+    </row>
+    <row r="55" spans="1:2" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="35" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="19.5" thickBot="1">
-      <c r="A55" s="37" t="s">
+      <c r="B55" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="B55" s="37" t="s">
+    </row>
+    <row r="56" spans="1:2" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="36" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="19">
-      <c r="A56" s="38" t="s">
+      <c r="B56" s="36" t="s">
         <v>262</v>
-      </c>
-      <c r="B56" s="38" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>